<commit_message>
skos vocabulary for dmcar - 1st draft complete
</commit_message>
<xml_diff>
--- a/dmcar_skos_vocabulary.xlsx
+++ b/dmcar_skos_vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="136">
   <si>
     <t xml:space="preserve">ConceptScheme</t>
   </si>
@@ -378,46 +378,82 @@
     <t xml:space="preserve">Index</t>
   </si>
   <si>
+    <t xml:space="preserve">An index is a database structure that defines the creation of pointers and lookups that can be used by a query engine to define query plans that optimise performance.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Constraint</t>
   </si>
   <si>
+    <t xml:space="preserve">A constraint is a rule imposed on data in a table at column level, constraining the values that can be legally populated whilst preserving database integrity. Different rules might stipulare uniqueness, or the avoidance of null values. Foreign key constrains enforce that a value placed in the column match one of the primary key values from a lookup table. Different database platforms will offer a range of constraint options.</t>
+  </si>
+  <si>
     <t xml:space="preserve">CompoundKey</t>
   </si>
   <si>
     <t xml:space="preserve">Compound Key</t>
   </si>
   <si>
+    <t xml:space="preserve">A compound key is some link between tables that requires more than a single key. This might be because the primary key on the lookup table is a compound primary key, or it might be an unusual type of join. In most situations, compound keys can be replaced with a simpler, more performant type of database link and their adoption should be carefully considered.</t>
+  </si>
+  <si>
     <t xml:space="preserve">PrimaryKey, ForeignKey</t>
   </si>
   <si>
     <t xml:space="preserve">KGNAM</t>
   </si>
   <si>
+    <t xml:space="preserve">KGNAM is the namespace prefix for the kgnaming ontology. This ontology formalises some expectations around what information can be expected to be provided for a “NamedObject”. This would tend to include, a name, a “FullyQualifiedName” that can be used for mastering, and other common properties to enable certain features of a knowledge graph platform.</t>
+  </si>
+  <si>
     <t xml:space="preserve">DMCAR</t>
   </si>
   <si>
+    <t xml:space="preserve">DMCAR is the namespace prefix for the kgdmcar ontology. This ontology focuses on the main entities and interactions found within the Data Modelling domain, and aims to enable the capture of data modelling information to a high degree of fidelity.</t>
+  </si>
+  <si>
     <t xml:space="preserve">NamedObject</t>
   </si>
   <si>
     <t xml:space="preserve">Named Object</t>
   </si>
   <si>
+    <t xml:space="preserve">A NamedObject is a concept inherited from the kgnaming ontology. It defines some object, concept or thing that has a name, and a fully-qualified-name that enables that object to be uniquely identified. Additionally, NamedObjects are expected to have Descriptions and Labels to provide additional context.</t>
+  </si>
+  <si>
     <t xml:space="preserve">FullyQualifiedName</t>
   </si>
   <si>
     <t xml:space="preserve">Fully Qualified Name</t>
   </si>
   <si>
+    <t xml:space="preserve">A fully qualified name is a name that uniquely and unambiguously identifies an object. It is constructed by prepending an object’s namespace prior to the objects (short) name, separated by a dot. In some instances, namespaces can be compounded, with each level of namespace being delimited by a dot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NamedObject, KGNAM, Name</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
+    <t xml:space="preserve">A description is a passage of text whose purpose is to outline what the associated object is, and provide additional contextual information. A good description should help someone’s understanding of an object.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
+    <t xml:space="preserve">A name is a string of text that conforms to some constraints that can be used to identify an object. Some names are used colloquially and are not always formalised, resulting in possible “punning” or ambiguity. Main constrains in name-construction are no whitespace, and avoidance of dots, commas and other punctuation.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Label</t>
   </si>
   <si>
+    <t xml:space="preserve">A label is a relatively unconstricted string used to label an object. A label can contain dots, commas and whitespace. It may be used in visualisations or on gui components, so some care should be applied in choosing appropriate labels.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An interface is a specification that enables data be transferred or communicated between containers. Most interfaces will expose a schema, and publish details about how it will interpret, or expect that schema to be interpreted. </t>
   </si>
 </sst>
 </file>
@@ -730,8 +766,8 @@
   </sheetPr>
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K47" activeCellId="0" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1349,7 +1385,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
@@ -1359,118 +1395,160 @@
       <c r="D37" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>111</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>122</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>125</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>128</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>130</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates in prep for multivalues capability in serialisation process
</commit_message>
<xml_diff>
--- a/dmcar_skos_vocabulary.xlsx
+++ b/dmcar_skos_vocabulary.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">SeeAlso</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Modelling</t>
+    <t xml:space="preserve">DataModelling</t>
   </si>
   <si>
     <t xml:space="preserve">Namespace</t>
@@ -296,32 +296,7 @@
     <t xml:space="preserve">Data-Type Scheme</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">A Datatype scheme is a vocabulary of datatypes that might be used in a given context. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Commonly, collections of datatype specifications will be grouped into a Datatype Scheme to form a recognisable standard. These could be proprietary to d</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ifferent standards bodies, database platforms, languages and data format specifications.</t>
-    </r>
+    <t xml:space="preserve">A Datatype scheme is a vocabulary of datatypes that might be used in a given context. Commonly, collections of datatype specifications will be grouped into a Datatype Scheme to form a recognisable standard. These could be proprietary to different standards bodies, database platforms, languages and data format specifications.</t>
   </si>
   <si>
     <t xml:space="preserve">DataType</t>
@@ -463,7 +438,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -497,11 +472,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -766,8 +736,8 @@
   </sheetPr>
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K47" activeCellId="0" sqref="K47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1283,7 +1253,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
serialisation complete + renaming kg-ontologies to follow the kgraph.foo domain namespace
</commit_message>
<xml_diff>
--- a/dmcar_skos_vocabulary.xlsx
+++ b/dmcar_skos_vocabulary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
   <si>
     <t xml:space="preserve">ConceptScheme</t>
   </si>
@@ -101,6 +101,9 @@
     <t xml:space="preserve">A schema is a foundational data structure defining attributes with associated types and constraints. It’s a broad concept encompassing class, entity, and table definitions, extending to dynamic data like messages and query results. Schemas often exhibit relaxed normalization, prioritizing flexibility across diverse data representations.</t>
   </si>
   <si>
+    <t xml:space="preserve">Class, Table, Interface</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
     <t xml:space="preserve">A Class describes some set of objects that can be considered the same. That is, they can all be expected to share the same set of associated attributes and relationships by virtue of their being members of the class.</t>
   </si>
   <si>
+    <t xml:space="preserve">Schema, Table, Interface</t>
+  </si>
+  <si>
     <t xml:space="preserve">Join</t>
   </si>
   <si>
@@ -167,6 +173,9 @@
     <t xml:space="preserve">A table is a physical embodyment of a class in a relational database. A table will have a number of attributes associated with it expressed as columns, and individual instances of the entities modelled by the table will be expressed as rows of the table.</t>
   </si>
   <si>
+    <t xml:space="preserve">Schema, Class, Interface</t>
+  </si>
+  <si>
     <t xml:space="preserve">A concept is a unit or topic of thought.</t>
   </si>
   <si>
@@ -185,7 +194,7 @@
     <t xml:space="preserve">Dataset</t>
   </si>
   <si>
-    <t xml:space="preserve">A dataset is a curated collection of interrelated data, structured according to a defined data model and constrained by some set of specific scoping criteria – perhaps expressed as a series of temporal, geographical, or sourcing constraints. </t>
+    <t xml:space="preserve">A dataset is a curated collection of interrelated data, structured according to a defined data model and constrained (either formally, or by practical consequence) by some set of specific scoping criteria – these could be for example, temporal, geographical, or practical sourcing constraints or a combination of these and more.</t>
   </si>
   <si>
     <t xml:space="preserve">Row</t>
@@ -429,6 +438,9 @@
   </si>
   <si>
     <t xml:space="preserve">An interface is a specification that enables data be transferred or communicated between containers. Most interfaces will expose a schema, and publish details about how it will interpret, or expect that schema to be interpreted. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schema, Class, Table</t>
   </si>
 </sst>
 </file>
@@ -736,8 +748,8 @@
   </sheetPr>
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K48" activeCellId="0" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -871,22 +883,25 @@
       <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="K6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,13 +909,13 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -908,16 +923,19 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -925,13 +943,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,19 +957,19 @@
         <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,19 +977,19 @@
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,13 +997,16 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -999,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,13 +1028,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,27 +1042,27 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,16 +1070,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1066,13 +1087,13 @@
         <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1080,13 +1101,13 @@
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,16 +1115,16 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1111,13 +1132,13 @@
         <v>14</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1125,19 +1146,19 @@
         <v>14</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,13 +1166,13 @@
         <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>21</v>
@@ -1162,13 +1183,13 @@
         <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>21</v>
@@ -1179,13 +1200,13 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>21</v>
@@ -1196,13 +1217,13 @@
         <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,13 +1231,13 @@
         <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1224,16 +1245,16 @@
         <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1241,16 +1262,16 @@
         <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,13 +1279,13 @@
         <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,13 +1293,13 @@
         <v>14</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,16 +1307,16 @@
         <v>14</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1303,16 +1324,16 @@
         <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,19 +1341,19 @@
         <v>14</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1340,19 +1361,19 @@
         <v>14</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1360,13 +1381,13 @@
         <v>14</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,13 +1395,13 @@
         <v>14</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,16 +1409,16 @@
         <v>14</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1405,13 +1426,13 @@
         <v>14</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,13 +1440,13 @@
         <v>14</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,13 +1454,13 @@
         <v>14</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,16 +1468,16 @@
         <v>14</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1464,13 +1485,13 @@
         <v>14</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,16 +1499,16 @@
         <v>14</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,13 +1516,13 @@
         <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1509,16 +1530,16 @@
         <v>14</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>